<commit_message>
New and improved search pattern
</commit_message>
<xml_diff>
--- a/doc/Behaviour/HeadBehaviourPoints.xlsx
+++ b/doc/Behaviour/HeadBehaviourPoints.xlsx
@@ -88,8 +88,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -104,17 +124,37 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -155,90 +195,84 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$28</c:f>
+              <c:f>Sheet1!$A$1:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.5</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.5</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.5</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.25</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.25</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.25</c:v>
+                  <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25</c:v>
+                  <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.0</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$28</c:f>
+              <c:f>Sheet1!$B$1:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.0</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-1.0</c:v>
@@ -253,34 +287,28 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.5</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>-0.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-1.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,7 +320,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$35</c:f>
+              <c:f>Sheet1!$D$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -303,7 +331,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$I$35</c:f>
+              <c:f>Sheet1!$E$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -327,7 +355,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$36:$I$36</c:f>
+              <c:f>Sheet1!$E$33:$I$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -417,13 +445,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -768,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection sqref="A1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -781,7 +809,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>-0.5</v>
@@ -789,23 +817,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>-1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="B4">
         <v>-0.5</v>
@@ -813,15 +841,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
         <v>-0.5</v>
-      </c>
-      <c r="B5">
-        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -829,7 +857,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>-0.25</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>-0.5</v>
@@ -837,7 +865,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>-0.25</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -845,7 +873,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -856,28 +884,28 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
+        <v>-0.5</v>
+      </c>
+      <c r="B11">
         <v>0</v>
-      </c>
-      <c r="B11">
-        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="B12">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="B13">
         <v>-0.5</v>
@@ -885,160 +913,144 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="B16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>-0.25</v>
+      </c>
+      <c r="B17">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>0.5</v>
-      </c>
-      <c r="B17">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
+    <row r="20" spans="1:9">
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1.0471999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="D21" t="s">
         <v>1</v>
       </c>
-      <c r="B18">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E21">
+        <v>0.78539800000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="D23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>1.0471999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>0.78539800000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26">
         <f xml:space="preserve"> 4 * PI() / 3</f>
         <v>4.1887902047863905</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="D27" t="s">
+    <row r="24" spans="1:9">
+      <c r="D24" t="s">
         <v>3</v>
       </c>
-      <c r="E27">
+      <c r="E24">
         <f xml:space="preserve"> 2 * PI() / 3</f>
         <v>2.0943951023931953</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="26" spans="1:9">
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f>E20/E23</f>
+        <v>0.25000058460874919</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="E27">
+        <f>E21/E24</f>
+        <v>0.37499992198346532</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="D29" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E29">
-        <f>E23/E26</f>
+        <f>E26</f>
         <v>0.25000058460874919</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:9">
       <c r="E30">
-        <f>E24/E27</f>
+        <f>E27</f>
         <v>0.37499992198346532</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:9">
       <c r="D32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32">
-        <f>E29</f>
+        <f>$E29</f>
         <v>0.25000058460874919</v>
       </c>
-    </row>
-    <row r="33" spans="4:9">
+      <c r="F32">
+        <f>-$E29</f>
+        <v>-0.25000058460874919</v>
+      </c>
+      <c r="G32">
+        <f>-$E29</f>
+        <v>-0.25000058460874919</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ref="H32" si="0">$E29</f>
+        <v>0.25000058460874919</v>
+      </c>
+      <c r="I32">
+        <f>$E29</f>
+        <v>0.25000058460874919</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9">
       <c r="E33">
-        <f>E30</f>
+        <f>$E30</f>
         <v>0.37499992198346532</v>
       </c>
-    </row>
-    <row r="35" spans="4:9">
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35">
-        <f>$E32</f>
-        <v>0.25000058460874919</v>
-      </c>
-      <c r="F35">
-        <f>-$E32</f>
-        <v>-0.25000058460874919</v>
-      </c>
-      <c r="G35">
-        <f>-$E32</f>
-        <v>-0.25000058460874919</v>
-      </c>
-      <c r="H35">
-        <f t="shared" ref="H35" si="0">$E32</f>
-        <v>0.25000058460874919</v>
-      </c>
-      <c r="I35">
-        <f>$E32</f>
-        <v>0.25000058460874919</v>
-      </c>
-    </row>
-    <row r="36" spans="4:9">
-      <c r="E36">
-        <f>$E33</f>
+      <c r="F33">
+        <f>$E30</f>
         <v>0.37499992198346532</v>
       </c>
-      <c r="F36">
-        <f>$E33</f>
-        <v>0.37499992198346532</v>
-      </c>
-      <c r="G36">
-        <f>-$E33</f>
+      <c r="G33">
+        <f>-$E30</f>
         <v>-0.37499992198346532</v>
       </c>
-      <c r="H36">
-        <f>-$E33</f>
+      <c r="H33">
+        <f>-$E30</f>
         <v>-0.37499992198346532</v>
       </c>
-      <c r="I36">
-        <f>$E33</f>
+      <c r="I33">
+        <f>$E30</f>
         <v>0.37499992198346532</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New head behaviour params. Now fixate longer and search higher
</commit_message>
<xml_diff>
--- a/doc/Behaviour/HeadBehaviourPoints.xlsx
+++ b/doc/Behaviour/HeadBehaviourPoints.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Search after Game1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>FOV_X</t>
   </si>
@@ -88,8 +89,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -124,7 +129,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -140,6 +145,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -155,6 +162,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,6 +448,295 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:tailEnd type="arrow"/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Search after Game1'!$A$1:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Search after Game1'!$B$1:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Search after Game1'!$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>points:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Search after Game1'!$E$30:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.250000584608749</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.250000584608749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.250000584608749</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.250000584608749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.250000584608749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Search after Game1'!$E$31:$I$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.374999921983465</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.374999921983465</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.374999921983465</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.374999921983465</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.374999921983465</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2097437880"/>
+        <c:axId val="-2090120920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2097437880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090120920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2090120920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2097437880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -458,6 +756,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -798,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:B17"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1051,6 +1386,290 @@
       </c>
       <c r="I33">
         <f>$E30</f>
+        <v>0.37499992198346532</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>0.25</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>0.25</v>
+      </c>
+      <c r="B4">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>0.75</v>
+      </c>
+      <c r="B8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>0.25</v>
+      </c>
+      <c r="B10">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>-0.25</v>
+      </c>
+      <c r="B12">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>-0.5</v>
+      </c>
+      <c r="B13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>-0.75</v>
+      </c>
+      <c r="B14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>-1</v>
+      </c>
+      <c r="B15">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>-0.5</v>
+      </c>
+      <c r="B16">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>-0.5</v>
+      </c>
+      <c r="B17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>-0.25</v>
+      </c>
+      <c r="B18">
+        <v>-1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1.0471999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>-0.25</v>
+      </c>
+      <c r="B19">
+        <v>-0.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.78539800000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <f xml:space="preserve"> 4 * PI() / 3</f>
+        <v>4.1887902047863905</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f xml:space="preserve"> 2 * PI() / 3</f>
+        <v>2.0943951023931953</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f>E18/E21</f>
+        <v>0.25000058460874919</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="E25">
+        <f>E19/E22</f>
+        <v>0.37499992198346532</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <f>E24</f>
+        <v>0.25000058460874919</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="E28">
+        <f>E25</f>
+        <v>0.37499992198346532</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <f>$E27</f>
+        <v>0.25000058460874919</v>
+      </c>
+      <c r="F30">
+        <f>-$E27</f>
+        <v>-0.25000058460874919</v>
+      </c>
+      <c r="G30">
+        <f>-$E27</f>
+        <v>-0.25000058460874919</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ref="H30" si="0">$E27</f>
+        <v>0.25000058460874919</v>
+      </c>
+      <c r="I30">
+        <f>$E27</f>
+        <v>0.25000058460874919</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="E31">
+        <f>$E28</f>
+        <v>0.37499992198346532</v>
+      </c>
+      <c r="F31">
+        <f>$E28</f>
+        <v>0.37499992198346532</v>
+      </c>
+      <c r="G31">
+        <f>-$E28</f>
+        <v>-0.37499992198346532</v>
+      </c>
+      <c r="H31">
+        <f>-$E28</f>
+        <v>-0.37499992198346532</v>
+      </c>
+      <c r="I31">
+        <f>$E28</f>
         <v>0.37499992198346532</v>
       </c>
     </row>

</xml_diff>